<commit_message>
case-control analysis for study periods.
</commit_message>
<xml_diff>
--- a/data/variant_study_case_control_COVID_data_ff_20220518.xlsx
+++ b/data/variant_study_case_control_COVID_data_ff_20220518.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fouziafarooq/Library/CloudStorage/Box-Box/1.GWU/R/COVID_Variant_Study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803CF3C3-FCD8-FA4E-AFE5-FA7B223017D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06FFCA8-AF0D-7C4A-B176-A982939B9EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="-20220" windowWidth="28040" windowHeight="16940" xr2:uid="{C20F5C01-24DE-1246-B7B9-8129ED3502B0}"/>
+    <workbookView xWindow="600" yWindow="-20220" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{C20F5C01-24DE-1246-B7B9-8129ED3502B0}"/>
   </bookViews>
   <sheets>
     <sheet name="country-date" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Dates" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -603,7 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C8411F-C1D9-B344-B9F7-D2063000A864}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
@@ -2050,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F4AA11-B446-DD4E-9B5B-F7C2B73DECDF}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>